<commit_message>
Add FSW, DCP, and coh_int fields to L1 files
</commit_message>
<xml_diff>
--- a/dat/L1_Dict/L1_Dict_v2_4.xlsx
+++ b/dat/L1_Dict/L1_Dict_v2_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlav736\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlav736\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A844FD-4812-440C-B751-9E98604566CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AB21E-88F9-4D95-B7A4-5F610EB55115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="469">
   <si>
     <t>Comment</t>
   </si>
@@ -1455,12 +1455,21 @@
   <si>
     <t>longitude</t>
   </si>
+  <si>
+    <t>coh_int</t>
+  </si>
+  <si>
+    <t>Coherent Integration time</t>
+  </si>
+  <si>
+    <t>Coherent integration time in seconds</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1477,6 +1486,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1517,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1533,6 +1549,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1814,11 +1833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X916"/>
+  <dimension ref="A1:X917"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L88" sqref="L88"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2993,24 +3012,24 @@
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
     </row>
-    <row r="30" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>28</v>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>468</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>1</v>
@@ -3033,12 +3052,12 @@
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>365</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>366</v>
+        <v>27</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>12</v>
@@ -3050,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>367</v>
+        <v>28</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>1</v>
@@ -3075,13 +3094,13 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>29</v>
+        <v>365</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1</v>
+        <v>366</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>1</v>
@@ -3090,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>30</v>
+        <v>367</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>1</v>
@@ -3115,7 +3134,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>1</v>
@@ -3130,7 +3149,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>1</v>
@@ -3155,7 +3174,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>333</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>1</v>
@@ -3170,7 +3189,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>1</v>
@@ -3195,7 +3214,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>1</v>
@@ -3210,7 +3229,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>1</v>
@@ -3235,7 +3254,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>385</v>
+        <v>334</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>1</v>
@@ -3250,7 +3269,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>386</v>
+        <v>46</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>1</v>
@@ -3275,7 +3294,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>327</v>
+        <v>385</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>1</v>
@@ -3290,7 +3309,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>328</v>
+        <v>386</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>1</v>
@@ -3315,7 +3334,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>33</v>
+        <v>327</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>1</v>
@@ -3330,7 +3349,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>34</v>
+        <v>328</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>1</v>
@@ -3355,7 +3374,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>1</v>
@@ -3370,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>1</v>
@@ -3395,7 +3414,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>1</v>
@@ -3410,7 +3429,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>1</v>
@@ -3435,7 +3454,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>1</v>
@@ -3450,7 +3469,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>1</v>
@@ -3475,7 +3494,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>1</v>
@@ -3490,7 +3509,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>1</v>
@@ -3515,7 +3534,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>1</v>
@@ -3530,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>1</v>
@@ -3555,7 +3574,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>1</v>
@@ -3570,7 +3589,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>1</v>
@@ -3593,24 +3612,24 @@
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
     </row>
-    <row r="45" spans="1:24" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>342</v>
+        <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>320</v>
+        <v>48</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>1</v>
@@ -3633,24 +3652,24 @@
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>330</v>
+        <v>51</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>55</v>
+        <v>320</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>1</v>
@@ -3673,24 +3692,24 @@
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
     </row>
-    <row r="47" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>51</v>
+        <v>330</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>1</v>
@@ -3713,12 +3732,12 @@
       <c r="W47" s="2"/>
       <c r="X47" s="2"/>
     </row>
-    <row r="48" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>51</v>
@@ -3730,7 +3749,7 @@
         <v>342</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>1</v>
@@ -3753,24 +3772,24 @@
       <c r="W48" s="2"/>
       <c r="X48" s="2"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="63" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>330</v>
+        <v>51</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>1</v>
@@ -3795,22 +3814,22 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>51</v>
+        <v>330</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>1</v>
@@ -3833,24 +3852,24 @@
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
     </row>
-    <row r="51" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>342</v>
+        <v>66</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>350</v>
+        <v>67</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D51" s="4">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>351</v>
+        <v>68</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>1</v>
@@ -3875,22 +3894,22 @@
     </row>
     <row r="52" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>69</v>
+        <v>342</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>70</v>
+        <v>350</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>71</v>
+        <v>330</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>72</v>
+        <v>351</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>1</v>
@@ -3915,10 +3934,10 @@
     </row>
     <row r="53" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -3930,7 +3949,7 @@
         <v>342</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>1</v>
@@ -3955,10 +3974,10 @@
     </row>
     <row r="54" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>51</v>
@@ -3970,7 +3989,7 @@
         <v>342</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>1</v>
@@ -3995,22 +4014,22 @@
     </row>
     <row r="55" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>1</v>
@@ -4035,10 +4054,10 @@
     </row>
     <row r="56" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>51</v>
@@ -4050,7 +4069,7 @@
         <v>342</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>1</v>
@@ -4075,10 +4094,10 @@
     </row>
     <row r="57" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>51</v>
@@ -4090,7 +4109,7 @@
         <v>342</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>1</v>
@@ -4115,22 +4134,22 @@
     </row>
     <row r="58" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>1</v>
@@ -4155,10 +4174,10 @@
     </row>
     <row r="59" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>51</v>
@@ -4170,7 +4189,7 @@
         <v>342</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>1</v>
@@ -4195,10 +4214,10 @@
     </row>
     <row r="60" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>51</v>
@@ -4210,7 +4229,7 @@
         <v>342</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>1</v>
@@ -4235,22 +4254,22 @@
     </row>
     <row r="61" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>1</v>
@@ -4275,10 +4294,10 @@
     </row>
     <row r="62" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>51</v>
@@ -4290,7 +4309,7 @@
         <v>342</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>1</v>
@@ -4315,10 +4334,10 @@
     </row>
     <row r="63" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>51</v>
@@ -4330,7 +4349,7 @@
         <v>342</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>1</v>
@@ -4355,22 +4374,22 @@
     </row>
     <row r="64" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>332</v>
+        <v>51</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>1</v>
@@ -4395,10 +4414,10 @@
     </row>
     <row r="65" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>332</v>
@@ -4410,7 +4429,7 @@
         <v>342</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>1</v>
@@ -4435,10 +4454,10 @@
     </row>
     <row r="66" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>456</v>
+        <v>111</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>459</v>
+        <v>112</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>332</v>
@@ -4450,7 +4469,7 @@
         <v>342</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>460</v>
+        <v>113</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>1</v>
@@ -4475,10 +4494,10 @@
     </row>
     <row r="67" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>114</v>
+        <v>456</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>321</v>
+        <v>459</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>332</v>
@@ -4490,7 +4509,7 @@
         <v>342</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>115</v>
+        <v>460</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>1</v>
@@ -4515,10 +4534,10 @@
     </row>
     <row r="68" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>332</v>
@@ -4530,7 +4549,7 @@
         <v>342</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>1</v>
@@ -4555,10 +4574,10 @@
     </row>
     <row r="69" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>457</v>
+        <v>116</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>458</v>
+        <v>322</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>332</v>
@@ -4570,7 +4589,7 @@
         <v>342</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>461</v>
+        <v>117</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>1</v>
@@ -4593,27 +4612,27 @@
       <c r="W69" s="2"/>
       <c r="X69" s="2"/>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>118</v>
+        <v>457</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>119</v>
+        <v>458</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>51</v>
+        <v>332</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>121</v>
+        <v>461</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>464</v>
+        <v>1</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -4635,25 +4654,25 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -4675,25 +4694,25 @@
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>332</v>
+        <v>51</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>1</v>
+        <v>465</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -4713,24 +4732,24 @@
       <c r="W72" s="2"/>
       <c r="X72" s="2"/>
     </row>
-    <row r="73" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>51</v>
+        <v>332</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>1</v>
@@ -4755,22 +4774,22 @@
     </row>
     <row r="74" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>332</v>
+        <v>51</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>1</v>
@@ -4795,22 +4814,22 @@
     </row>
     <row r="75" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>335</v>
+        <v>133</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>337</v>
+        <v>134</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>1</v>
@@ -4835,22 +4854,22 @@
     </row>
     <row r="76" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>137</v>
+        <v>335</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>138</v>
+        <v>337</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>1</v>
@@ -4875,22 +4894,22 @@
     </row>
     <row r="77" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>336</v>
+        <v>137</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>338</v>
+        <v>138</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>1</v>
@@ -4913,24 +4932,24 @@
       <c r="W77" s="2"/>
       <c r="X77" s="2"/>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>141</v>
+        <v>336</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>142</v>
+        <v>338</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>143</v>
+        <v>332</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>1</v>
@@ -4955,10 +4974,10 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>143</v>
@@ -4970,7 +4989,7 @@
         <v>342</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>1</v>
@@ -4993,24 +5012,24 @@
       <c r="W79" s="2"/>
       <c r="X79" s="2"/>
     </row>
-    <row r="80" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>332</v>
+        <v>143</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>438</v>
+        <v>148</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>1</v>
@@ -5033,24 +5052,24 @@
       <c r="W80" s="2"/>
       <c r="X80" s="2"/>
     </row>
-    <row r="81" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>342</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>153</v>
+        <v>438</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>1</v>
@@ -5073,24 +5092,24 @@
       <c r="W81" s="2"/>
       <c r="X81" s="2"/>
     </row>
-    <row r="82" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>352</v>
+        <v>151</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>353</v>
+        <v>152</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D82" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>354</v>
+        <v>153</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>1</v>
@@ -5115,10 +5134,10 @@
     </row>
     <row r="83" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>154</v>
+        <v>352</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>155</v>
+        <v>353</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>329</v>
@@ -5127,10 +5146,10 @@
         <v>1</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>1</v>
@@ -5153,12 +5172,12 @@
       <c r="W83" s="2"/>
       <c r="X83" s="2"/>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>329</v>
@@ -5170,7 +5189,7 @@
         <v>343</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>158</v>
+        <v>349</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>1</v>
@@ -5193,15 +5212,15 @@
       <c r="W84" s="2"/>
       <c r="X84" s="2"/>
     </row>
-    <row r="85" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D85" s="4">
         <v>1</v>
@@ -5210,7 +5229,7 @@
         <v>343</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>1</v>
@@ -5233,24 +5252,24 @@
       <c r="W85" s="2"/>
       <c r="X85" s="2"/>
     </row>
-    <row r="86" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D86" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D86" s="4">
         <v>1</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>1</v>
@@ -5273,24 +5292,24 @@
       <c r="W86" s="2"/>
       <c r="X86" s="2"/>
     </row>
-    <row r="87" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D87" s="4">
+        <v>329</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>1</v>
@@ -5315,10 +5334,10 @@
     </row>
     <row r="88" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>332</v>
@@ -5330,7 +5349,7 @@
         <v>343</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>438</v>
+        <v>167</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>1</v>
@@ -5355,16 +5374,16 @@
     </row>
     <row r="89" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>25</v>
+      <c r="D89" s="4">
+        <v>1</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>343</v>
@@ -5395,16 +5414,16 @@
     </row>
     <row r="90" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D90" s="4">
-        <v>1</v>
+      <c r="D90" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>343</v>
@@ -5435,10 +5454,10 @@
     </row>
     <row r="91" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>332</v>
@@ -5475,16 +5494,16 @@
     </row>
     <row r="92" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>360</v>
+        <v>175</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>25</v>
+      <c r="D92" s="4">
+        <v>1</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>343</v>
@@ -5515,16 +5534,16 @@
     </row>
     <row r="93" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>178</v>
+        <v>360</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D93" s="4">
-        <v>1</v>
+      <c r="D93" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>343</v>
@@ -5555,10 +5574,10 @@
     </row>
     <row r="94" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>332</v>
@@ -5595,16 +5614,16 @@
     </row>
     <row r="95" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>25</v>
+      <c r="D95" s="4">
+        <v>1</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>343</v>
@@ -5635,22 +5654,22 @@
     </row>
     <row r="96" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>185</v>
+        <v>438</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>1</v>
@@ -5673,27 +5692,27 @@
       <c r="W96" s="2"/>
       <c r="X96" s="2"/>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>51</v>
+        <v>332</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>464</v>
+        <v>1</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -5715,25 +5734,25 @@
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -5753,27 +5772,27 @@
       <c r="W98" s="2"/>
       <c r="X98" s="2"/>
     </row>
-    <row r="99" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>332</v>
+        <v>51</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>1</v>
+        <v>465</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -5793,15 +5812,15 @@
       <c r="W99" s="2"/>
       <c r="X99" s="2"/>
     </row>
-    <row r="100" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>51</v>
+        <v>332</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>71</v>
@@ -5810,7 +5829,7 @@
         <v>343</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>1</v>
@@ -5835,10 +5854,10 @@
     </row>
     <row r="101" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>51</v>
@@ -5850,7 +5869,7 @@
         <v>343</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G101" s="4" t="s">
         <v>1</v>
@@ -5875,10 +5894,10 @@
     </row>
     <row r="102" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>51</v>
@@ -5890,7 +5909,7 @@
         <v>343</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>1</v>
@@ -5915,22 +5934,22 @@
     </row>
     <row r="103" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G103" s="4" t="s">
         <v>1</v>
@@ -5955,10 +5974,10 @@
     </row>
     <row r="104" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>51</v>
@@ -5970,7 +5989,7 @@
         <v>343</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>1</v>
@@ -5995,10 +6014,10 @@
     </row>
     <row r="105" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>51</v>
@@ -6010,7 +6029,7 @@
         <v>343</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G105" s="4" t="s">
         <v>1</v>
@@ -6035,22 +6054,22 @@
     </row>
     <row r="106" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>387</v>
+        <v>210</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>358</v>
+        <v>211</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D106" s="4">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>359</v>
+        <v>212</v>
       </c>
       <c r="G106" s="4" t="s">
         <v>1</v>
@@ -6073,24 +6092,24 @@
       <c r="W106" s="2"/>
       <c r="X106" s="2"/>
     </row>
-    <row r="107" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>213</v>
+        <v>387</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>214</v>
+        <v>358</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>215</v>
+        <v>329</v>
+      </c>
+      <c r="D107" s="4">
+        <v>1</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>216</v>
+        <v>359</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>1</v>
@@ -6113,12 +6132,12 @@
       <c r="W107" s="2"/>
       <c r="X107" s="2"/>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>368</v>
+        <v>213</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>369</v>
+        <v>214</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>332</v>
@@ -6130,7 +6149,7 @@
         <v>343</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>370</v>
+        <v>216</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>1</v>
@@ -6153,12 +6172,12 @@
       <c r="W108" s="2"/>
       <c r="X108" s="2"/>
     </row>
-    <row r="109" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>217</v>
+        <v>368</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>218</v>
+        <v>369</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>332</v>
@@ -6170,7 +6189,7 @@
         <v>343</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>323</v>
+        <v>370</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>1</v>
@@ -6193,12 +6212,12 @@
       <c r="W109" s="2"/>
       <c r="X109" s="2"/>
     </row>
-    <row r="110" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>332</v>
@@ -6210,7 +6229,7 @@
         <v>343</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>1</v>
@@ -6233,12 +6252,12 @@
       <c r="W110" s="2"/>
       <c r="X110" s="2"/>
     </row>
-    <row r="111" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" ht="63" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>332</v>
@@ -6250,7 +6269,7 @@
         <v>343</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>1</v>
@@ -6273,12 +6292,12 @@
       <c r="W111" s="2"/>
       <c r="X111" s="2"/>
     </row>
-    <row r="112" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>332</v>
@@ -6290,7 +6309,7 @@
         <v>343</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>1</v>
@@ -6313,24 +6332,24 @@
       <c r="W112" s="2"/>
       <c r="X112" s="2"/>
     </row>
-    <row r="113" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" ht="63" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>374</v>
+        <v>223</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>377</v>
+        <v>191</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>378</v>
+        <v>326</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>1</v>
@@ -6355,10 +6374,10 @@
     </row>
     <row r="114" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>332</v>
@@ -6370,7 +6389,7 @@
         <v>343</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>1</v>
@@ -6393,24 +6412,24 @@
       <c r="W114" s="2"/>
       <c r="X114" s="2"/>
     </row>
-    <row r="115" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D115" s="4">
-        <v>1</v>
+      <c r="D115" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>1</v>
@@ -6435,22 +6454,22 @@
     </row>
     <row r="116" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>225</v>
+        <v>361</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>226</v>
+        <v>362</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D116" s="4" t="s">
-        <v>227</v>
+      <c r="D116" s="4">
+        <v>1</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>228</v>
+        <v>380</v>
       </c>
       <c r="G116" s="4" t="s">
         <v>1</v>
@@ -6473,24 +6492,24 @@
       <c r="W116" s="2"/>
       <c r="X116" s="2"/>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G117" s="4" t="s">
         <v>1</v>
@@ -6515,22 +6534,22 @@
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>1</v>
@@ -6553,24 +6572,24 @@
       <c r="W118" s="2"/>
       <c r="X118" s="2"/>
     </row>
-    <row r="119" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G119" s="4" t="s">
         <v>1</v>
@@ -6593,24 +6612,24 @@
       <c r="W119" s="2"/>
       <c r="X119" s="2"/>
     </row>
-    <row r="120" spans="1:24" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>451</v>
+        <v>236</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>452</v>
+        <v>237</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D120" s="4">
-        <v>1</v>
+      <c r="D120" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>454</v>
+        <v>238</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>1</v>
@@ -6633,12 +6652,12 @@
       <c r="W120" s="2"/>
       <c r="X120" s="2"/>
     </row>
-    <row r="121" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>332</v>
@@ -6650,7 +6669,7 @@
         <v>343</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>1</v>
@@ -6675,22 +6694,22 @@
     </row>
     <row r="122" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>239</v>
+        <v>448</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>240</v>
+        <v>449</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D122" s="4" t="s">
-        <v>241</v>
+      <c r="D122" s="4">
+        <v>1</v>
       </c>
       <c r="E122" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>1</v>
@@ -6713,24 +6732,24 @@
       <c r="W122" s="2"/>
       <c r="X122" s="2"/>
     </row>
-    <row r="123" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>437</v>
+        <v>241</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>1</v>
@@ -6753,24 +6772,24 @@
       <c r="W123" s="2"/>
       <c r="X123" s="2"/>
     </row>
-    <row r="124" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" ht="63" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>381</v>
+        <v>242</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>382</v>
+        <v>243</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D124" s="4">
-        <v>1</v>
+        <v>332</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>437</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>1</v>
@@ -6795,13 +6814,13 @@
     </row>
     <row r="125" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>244</v>
+        <v>381</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>245</v>
+        <v>382</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D125" s="4">
         <v>1</v>
@@ -6810,7 +6829,7 @@
         <v>343</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>246</v>
+        <v>453</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>1</v>
@@ -6833,24 +6852,24 @@
       <c r="W125" s="2"/>
       <c r="X125" s="2"/>
     </row>
-    <row r="126" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D126" s="4" t="s">
-        <v>241</v>
+      <c r="D126" s="4">
+        <v>1</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>363</v>
+        <v>246</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>1</v>
@@ -6873,24 +6892,24 @@
       <c r="W126" s="2"/>
       <c r="X126" s="2"/>
     </row>
-    <row r="127" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>51</v>
+        <v>332</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>71</v>
+        <v>241</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>251</v>
+        <v>363</v>
       </c>
       <c r="G127" s="4" t="s">
         <v>1</v>
@@ -6915,10 +6934,10 @@
     </row>
     <row r="128" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>51</v>
@@ -6930,7 +6949,7 @@
         <v>343</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>1</v>
@@ -6955,10 +6974,10 @@
     </row>
     <row r="129" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>51</v>
@@ -6970,7 +6989,7 @@
         <v>343</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>1</v>
@@ -6995,10 +7014,10 @@
     </row>
     <row r="130" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>51</v>
@@ -7010,7 +7029,7 @@
         <v>343</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G130" s="4" t="s">
         <v>1</v>
@@ -7035,10 +7054,10 @@
     </row>
     <row r="131" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>51</v>
@@ -7050,7 +7069,7 @@
         <v>343</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>1</v>
@@ -7075,22 +7094,22 @@
     </row>
     <row r="132" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E132" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G132" s="4" t="s">
         <v>1</v>
@@ -7115,10 +7134,10 @@
     </row>
     <row r="133" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>51</v>
@@ -7130,7 +7149,7 @@
         <v>343</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>1</v>
@@ -7155,10 +7174,10 @@
     </row>
     <row r="134" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>51</v>
@@ -7170,7 +7189,7 @@
         <v>343</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>1</v>
@@ -7193,24 +7212,24 @@
       <c r="W134" s="2"/>
       <c r="X134" s="2"/>
     </row>
-    <row r="135" spans="1:24" ht="63" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D135" s="4">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F135" s="4" t="s">
-        <v>439</v>
+        <v>272</v>
       </c>
       <c r="G135" s="4" t="s">
         <v>1</v>
@@ -7233,24 +7252,24 @@
       <c r="W135" s="2"/>
       <c r="X135" s="2"/>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" ht="63" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>347</v>
+        <v>273</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D136" s="4" t="s">
-        <v>215</v>
+      <c r="D136" s="4">
+        <v>1</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>276</v>
+        <v>439</v>
       </c>
       <c r="G136" s="4" t="s">
         <v>1</v>
@@ -7275,22 +7294,22 @@
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>277</v>
+        <v>347</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>71</v>
+        <v>215</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G137" s="4" t="s">
         <v>1</v>
@@ -7315,10 +7334,10 @@
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>332</v>
@@ -7330,7 +7349,7 @@
         <v>343</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G138" s="4" t="s">
         <v>1</v>
@@ -7355,22 +7374,22 @@
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>396</v>
+        <v>280</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>397</v>
+        <v>281</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D139" s="4">
-        <v>1</v>
+      <c r="D139" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>398</v>
+        <v>282</v>
       </c>
       <c r="G139" s="4" t="s">
         <v>1</v>
@@ -7395,22 +7414,22 @@
     </row>
     <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D140" s="4" t="s">
-        <v>283</v>
+      <c r="D140" s="4">
+        <v>1</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="G140" s="4" t="s">
         <v>1</v>
@@ -7433,24 +7452,24 @@
       <c r="W140" s="2"/>
       <c r="X140" s="2"/>
     </row>
-    <row r="141" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>284</v>
+        <v>393</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>285</v>
+        <v>394</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="D141" s="4">
-        <v>1</v>
+        <v>332</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="E141" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>286</v>
+        <v>395</v>
       </c>
       <c r="G141" s="4" t="s">
         <v>1</v>
@@ -7475,10 +7494,10 @@
     </row>
     <row r="142" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>329</v>
@@ -7490,7 +7509,7 @@
         <v>343</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G142" s="4" t="s">
         <v>1</v>
@@ -7515,13 +7534,13 @@
     </row>
     <row r="143" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D143" s="4">
         <v>1</v>
@@ -7530,7 +7549,7 @@
         <v>343</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>440</v>
+        <v>289</v>
       </c>
       <c r="G143" s="4" t="s">
         <v>1</v>
@@ -7555,10 +7574,10 @@
     </row>
     <row r="144" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>332</v>
@@ -7570,7 +7589,7 @@
         <v>343</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G144" s="4" t="s">
         <v>1</v>
@@ -7593,12 +7612,12 @@
       <c r="W144" s="2"/>
       <c r="X144" s="2"/>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>345</v>
+        <v>292</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>346</v>
+        <v>293</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>332</v>
@@ -7610,7 +7629,7 @@
         <v>343</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>346</v>
+        <v>441</v>
       </c>
       <c r="G145" s="4" t="s">
         <v>1</v>
@@ -7633,15 +7652,15 @@
       <c r="W145" s="2"/>
       <c r="X145" s="2"/>
     </row>
-    <row r="146" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>295</v>
+        <v>346</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D146" s="4">
         <v>1</v>
@@ -7650,7 +7669,7 @@
         <v>343</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>296</v>
+        <v>346</v>
       </c>
       <c r="G146" s="4" t="s">
         <v>1</v>
@@ -7675,22 +7694,22 @@
     </row>
     <row r="147" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>399</v>
+        <v>294</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>400</v>
+        <v>295</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>297</v>
+        <v>331</v>
+      </c>
+      <c r="D147" s="4">
+        <v>1</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>401</v>
+        <v>296</v>
       </c>
       <c r="G147" s="4" t="s">
         <v>1</v>
@@ -7715,22 +7734,22 @@
     </row>
     <row r="148" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D148" s="4">
-        <v>1</v>
+      <c r="D148" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F148" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G148" s="4" t="s">
         <v>1</v>
@@ -7753,15 +7772,15 @@
       <c r="W148" s="2"/>
       <c r="X148" s="2"/>
     </row>
-    <row r="149" spans="1:24" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D149" s="4">
         <v>1</v>
@@ -7770,7 +7789,7 @@
         <v>343</v>
       </c>
       <c r="F149" s="4" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="G149" s="4" t="s">
         <v>1</v>
@@ -7793,24 +7812,24 @@
       <c r="W149" s="2"/>
       <c r="X149" s="2"/>
     </row>
-    <row r="150" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>339</v>
+        <v>389</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>298</v>
+        <v>392</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D150" s="4" t="s">
-        <v>299</v>
+        <v>329</v>
+      </c>
+      <c r="D150" s="4">
+        <v>1</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F150" s="4" t="s">
-        <v>300</v>
+        <v>390</v>
       </c>
       <c r="G150" s="4" t="s">
         <v>1</v>
@@ -7835,22 +7854,22 @@
     </row>
     <row r="151" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>356</v>
+        <v>298</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D151" s="4">
-        <v>1</v>
+      <c r="D151" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>357</v>
+        <v>300</v>
       </c>
       <c r="G151" s="4" t="s">
         <v>1</v>
@@ -7873,24 +7892,24 @@
       <c r="W151" s="2"/>
       <c r="X151" s="2"/>
     </row>
-    <row r="152" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>301</v>
+        <v>356</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="D152" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D152" s="4">
         <v>1</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>343</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>462</v>
+        <v>357</v>
       </c>
       <c r="G152" s="4" t="s">
         <v>1</v>
@@ -7915,22 +7934,22 @@
     </row>
     <row r="153" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>302</v>
+        <v>364</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D153" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>371</v>
+        <v>462</v>
       </c>
       <c r="G153" s="4" t="s">
         <v>1</v>
@@ -7955,22 +7974,22 @@
     </row>
     <row r="154" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>455</v>
+        <v>302</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="D154" s="4" t="s">
-        <v>227</v>
+        <v>331</v>
+      </c>
+      <c r="D154" s="4">
+        <v>1</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>344</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G154" s="4" t="s">
         <v>1</v>
@@ -7995,22 +8014,22 @@
     </row>
     <row r="155" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>305</v>
+        <v>455</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>283</v>
+        <v>227</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>344</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>307</v>
+        <v>372</v>
       </c>
       <c r="G155" s="4" t="s">
         <v>1</v>
@@ -8033,12 +8052,12 @@
       <c r="W155" s="2"/>
       <c r="X155" s="2"/>
     </row>
-    <row r="156" spans="1:24" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>332</v>
@@ -8050,7 +8069,7 @@
         <v>344</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G156" s="4" t="s">
         <v>1</v>
@@ -8073,24 +8092,24 @@
       <c r="W156" s="2"/>
       <c r="X156" s="2"/>
     </row>
-    <row r="157" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>332</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="E157" s="4" t="s">
         <v>344</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G157" s="4" t="s">
         <v>1</v>
@@ -8115,22 +8134,22 @@
     </row>
     <row r="158" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="D158" s="4">
-        <v>1</v>
+      <c r="D158" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="F158" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G158" s="4" t="s">
         <v>1</v>
@@ -8153,12 +8172,28 @@
       <c r="W158" s="2"/>
       <c r="X158" s="2"/>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A159" s="2"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="F159" s="2"/>
-      <c r="G159" s="2"/>
+    <row r="159" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D159" s="4">
+        <v>1</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="G159" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
       <c r="J159" s="2"/>
@@ -8179,10 +8214,8 @@
     </row>
     <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
-      <c r="B160" s="2"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
@@ -27808,10 +27841,36 @@
       <c r="X914" s="2"/>
     </row>
     <row r="915" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A915" s="2"/>
       <c r="B915" s="2"/>
+      <c r="C915" s="2"/>
+      <c r="D915" s="2"/>
+      <c r="E915" s="2"/>
+      <c r="F915" s="2"/>
+      <c r="G915" s="2"/>
+      <c r="H915" s="2"/>
+      <c r="I915" s="2"/>
+      <c r="J915" s="2"/>
+      <c r="K915" s="2"/>
+      <c r="L915" s="2"/>
+      <c r="M915" s="2"/>
+      <c r="N915" s="2"/>
+      <c r="O915" s="2"/>
+      <c r="P915" s="2"/>
+      <c r="Q915" s="2"/>
+      <c r="R915" s="2"/>
+      <c r="S915" s="2"/>
+      <c r="T915" s="2"/>
+      <c r="U915" s="2"/>
+      <c r="V915" s="2"/>
+      <c r="W915" s="2"/>
+      <c r="X915" s="2"/>
     </row>
     <row r="916" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B916" s="2"/>
+    </row>
+    <row r="917" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B917" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>